<commit_message>
budget summary .PDF tdd step 3
</commit_message>
<xml_diff>
--- a/BOSSAPI/BossAPI/ooxml-table.xlsx
+++ b/BOSSAPI/BossAPI/ooxml-table.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>NFTM0317</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>11999623.00</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>13790687.00</t>
   </si>
 </sst>
 </file>
@@ -215,7 +224,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -561,6 +570,26 @@
         <v>52</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>